<commit_message>
Se agrego CARGA EMPLEADOS
</commit_message>
<xml_diff>
--- a/utils/docs/FORMATO_PARA_CARGAR_CLIENTES.xlsx
+++ b/utils/docs/FORMATO_PARA_CARGAR_CLIENTES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\aistermcon\utils\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93003C54-A61F-47D4-AEF2-439C63862448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF60EE2-53DB-4624-93F6-9DA3BE360C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,24 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>NOMBRE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>CLIENTES</t>
   </si>
   <si>
-    <t>RUC/CI</t>
-  </si>
-  <si>
-    <t>DIRECCION</t>
-  </si>
-  <si>
-    <t>TELEFONO</t>
-  </si>
-  <si>
-    <t>CORREO</t>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>RUC</t>
+  </si>
+  <si>
+    <t>CÉDULA</t>
+  </si>
+  <si>
+    <t>NOMBRE COMERCIAL</t>
+  </si>
+  <si>
+    <t>RAZÓN SOCIAL</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN</t>
+  </si>
+  <si>
+    <t>TELÉFONO</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
   </si>
 </sst>
 </file>
@@ -118,11 +127,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -404,43 +414,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" customFormat="1" ht="22.5">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="22.5">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -450,11 +470,20 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>